<commit_message>
Carga Aviso OK, Reporte OK, Colectivo NO OK, Actualiz Nomina NO OK, Nomina Actualizada 24-03-2022
</commit_message>
<xml_diff>
--- a/Git_Comandos_Utiles.xlsx
+++ b/Git_Comandos_Utiles.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bbracco\Documents\Python\RRHH\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FED92967-8A7E-4042-B526-8F41150A6BC6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54189143-1AC5-4C72-9110-BC1332AC7E3E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="27">
   <si>
     <t>Comando</t>
   </si>
@@ -166,6 +166,18 @@
   </si>
   <si>
     <t>Realiza un Add y Commit (Staging Area + Commit) en un solo paso</t>
+  </si>
+  <si>
+    <t>git config --global user.name</t>
+  </si>
+  <si>
+    <t>Devuelve el Nombre de Usuario de GIT</t>
+  </si>
+  <si>
+    <t>git status</t>
+  </si>
+  <si>
+    <t>Estado de los archivos</t>
   </si>
 </sst>
 </file>
@@ -237,8 +249,11 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{C5CE1550-7005-40E1-BA94-3080BEFA907E}" name="Tabla1" displayName="Tabla1" ref="A1:C9" totalsRowShown="0">
-  <autoFilter ref="A1:C9" xr:uid="{C5CE1550-7005-40E1-BA94-3080BEFA907E}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{C5CE1550-7005-40E1-BA94-3080BEFA907E}" name="Tabla1" displayName="Tabla1" ref="A1:C12" totalsRowShown="0">
+  <autoFilter ref="A1:C12" xr:uid="{C5CE1550-7005-40E1-BA94-3080BEFA907E}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C11">
+    <sortCondition ref="B1:B12"/>
+  </sortState>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{E86E477F-740B-4488-BA81-3688259A0C44}" name="Comando"/>
     <tableColumn id="3" xr3:uid="{9E441C25-3E95-4BD9-8BD1-2A26C15B4DC6}" name="Clasificacion"/>
@@ -511,10 +526,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C9"/>
+  <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -548,68 +563,68 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B3" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C3" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>9</v>
+        <v>23</v>
       </c>
       <c r="B4" t="s">
         <v>4</v>
       </c>
       <c r="C4" t="s">
-        <v>10</v>
+        <v>24</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>11</v>
+        <v>25</v>
       </c>
       <c r="B5" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C5" t="s">
-        <v>12</v>
+        <v>26</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>18</v>
+        <v>6</v>
       </c>
       <c r="B6" t="s">
         <v>7</v>
       </c>
       <c r="C6" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="B7" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="C7" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B8" t="s">
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="C8" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -621,6 +636,28 @@
       </c>
       <c r="C9" t="s">
         <v>22</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>16</v>
+      </c>
+      <c r="B10" t="s">
+        <v>14</v>
+      </c>
+      <c r="C10" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>17</v>
+      </c>
+      <c r="B11" t="s">
+        <v>19</v>
+      </c>
+      <c r="C11" t="s">
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
INGRESA NOVEDADES OK - REPORTE OK - NOMINA OK - COLECTIVO NO OK
</commit_message>
<xml_diff>
--- a/Git_Comandos_Utiles.xlsx
+++ b/Git_Comandos_Utiles.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bbracco\Documents\Python\RRHH\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E00C424E-1A3F-43EA-97F8-0236E3A1C1B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7409D5C6-3BEC-4082-8465-1D6467CC7151}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -536,7 +536,7 @@
   <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Funcionalidad 100% OK - Falta Login + Mejorar grafica de tablas + Descargar reportes
</commit_message>
<xml_diff>
--- a/Git_Comandos_Utiles.xlsx
+++ b/Git_Comandos_Utiles.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bbracco\Documents\Python\RRHH\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7409D5C6-3BEC-4082-8465-1D6467CC7151}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C09473A-BA83-401E-89F2-1A82B43937C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -216,12 +216,24 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -236,8 +248,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -536,7 +550,7 @@
   <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -561,7 +575,7 @@
       <c r="A2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C2" t="s">
@@ -572,7 +586,7 @@
       <c r="A3" t="s">
         <v>9</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C3" t="s">
@@ -583,7 +597,7 @@
       <c r="A4" t="s">
         <v>22</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C4" t="s">
@@ -594,7 +608,7 @@
       <c r="A5" t="s">
         <v>24</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C5" t="s">
@@ -605,7 +619,7 @@
       <c r="A6" t="s">
         <v>6</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="2" t="s">
         <v>7</v>
       </c>
       <c r="C6" t="s">
@@ -616,7 +630,7 @@
       <c r="A7" t="s">
         <v>11</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="2" t="s">
         <v>7</v>
       </c>
       <c r="C7" t="s">
@@ -627,7 +641,7 @@
       <c r="A8" t="s">
         <v>18</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="2" t="s">
         <v>7</v>
       </c>
       <c r="C8" t="s">
@@ -638,7 +652,7 @@
       <c r="A9" t="s">
         <v>20</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="2" t="s">
         <v>7</v>
       </c>
       <c r="C9" t="s">

</xml_diff>